<commit_message>
Update artefacts/Sprint 2 Artefacts/Unit Testing Records.xlsx
added my full name
</commit_message>
<xml_diff>
--- a/artefacts/Sprint 2 Artefacts/Unit Testing Records.xlsx
+++ b/artefacts/Sprint 2 Artefacts/Unit Testing Records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljh/Work/QUT/IFB299/Project/project_files/artefacts/Sprint 2 Artefacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC455540-6291-CE43-82C1-0D277C00F157}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18BE87E-D536-9847-8100-3E8C707BD3C6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Test Status</t>
-  </si>
-  <si>
-    <t>Jax</t>
   </si>
   <si>
     <t>User can login to their account successfully</t>
@@ -411,6 +408,9 @@
   <si>
     <t>Car Rental Project</t>
   </si>
+  <si>
+    <t>JianHong Lee (Jax)</t>
+  </si>
 </sst>
 </file>
 
@@ -604,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -679,6 +679,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,8 +1003,8 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1085,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="1"/>
@@ -1334,29 +1337,29 @@
       <c r="B10" s="9">
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1384,29 +1387,29 @@
       <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>17</v>
+      <c r="C11" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="J11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1434,29 +1437,29 @@
       <c r="B12" s="9">
         <v>5</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>17</v>
+      <c r="C12" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>33</v>
+      <c r="H12" s="9" t="s">
+        <v>31</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="J12" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1484,29 +1487,29 @@
       <c r="B13" s="9">
         <v>15</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>17</v>
+      <c r="C13" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="J13" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1534,29 +1537,29 @@
       <c r="B14" s="9">
         <v>15</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>17</v>
+      <c r="C14" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>35</v>
+      <c r="G14" s="9" t="s">
+        <v>36</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="I14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1584,29 +1587,29 @@
       <c r="B15" s="9">
         <v>15</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>17</v>
+      <c r="C15" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="I15" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1634,29 +1637,29 @@
       <c r="B16" s="9">
         <v>15</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>17</v>
+      <c r="C16" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>35</v>
+      <c r="G16" s="9" t="s">
+        <v>36</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="I16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1684,29 +1687,29 @@
       <c r="B17" s="11">
         <v>1</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>17</v>
+      <c r="C17" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>35</v>
+      <c r="G17" s="11" t="s">
+        <v>36</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="I17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -1734,29 +1737,29 @@
       <c r="B18" s="11">
         <v>10</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>17</v>
+      <c r="C18" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>56</v>
-      </c>
       <c r="H18" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -1784,29 +1787,29 @@
       <c r="B19" s="11">
         <v>10</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>17</v>
+      <c r="C19" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>58</v>
-      </c>
       <c r="G19" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -1835,28 +1838,28 @@
         <v>2</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>65</v>
-      </c>
       <c r="J20" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
@@ -1885,28 +1888,28 @@
         <v>2</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="J21" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -1935,28 +1938,28 @@
         <v>2</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>75</v>
-      </c>
       <c r="I22" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
@@ -1985,28 +1988,28 @@
         <v>2</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="I23" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
@@ -2035,28 +2038,28 @@
         <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="I24" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -2085,28 +2088,28 @@
         <v>1</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="I25" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2135,28 +2138,28 @@
         <v>7</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="F26" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="G26" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="H26" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>95</v>
-      </c>
       <c r="I26" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -2185,28 +2188,28 @@
         <v>16</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="H27" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="20" t="s">
-        <v>100</v>
-      </c>
       <c r="I27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>

</xml_diff>